<commit_message>
Generic text adder Added
</commit_message>
<xml_diff>
--- a/Excel/Akash.xlsx
+++ b/Excel/Akash.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Bikash Sharma</t>
   </si>
@@ -27,6 +27,18 @@
   </si>
   <si>
     <t>bikashsharma0775@gmail.com</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
   </si>
 </sst>
 </file>
@@ -371,40 +383,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="B3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="D1" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>